<commit_message>
[docs] 지갑 API 수정
</commit_message>
<xml_diff>
--- a/docs/API.xlsx
+++ b/docs/API.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\munseonghyun\Desktop\전달\개발일지\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Property\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CCA0C6-7D7D-498A-935D-B7892111F255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1D5B78B2-AC93-42EC-A552-EF922E2D665F}"/>
+    <workbookView xWindow="-110" yWindow="810" windowWidth="23260" windowHeight="12580" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="메인" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="마이페이지" sheetId="5" r:id="rId5"/>
     <sheet name="후기" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="156">
   <si>
     <t>api 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -741,11 +740,43 @@
     <t>login/user_findpass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>지갑 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지갑추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>myPage/addwallet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지갑주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ethaccount: ""</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
@@ -1027,11 +1058,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9751E270-2705-4C1D-BA28-67EDB4EC3EF9}" name="표1" displayName="표1" ref="B2:D19" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="B2:D19" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EFA8CC3C-6849-4319-A0D2-F88A57CC1A70}" name="depth"/>
-    <tableColumn id="2" xr3:uid="{E7A4A76E-234E-4CEE-B3AF-2C98343809CF}" name="depth2"/>
-    <tableColumn id="3" xr3:uid="{D19B786E-FBBC-4B95-B49C-886BBA1F6B2E}" name="depth3"/>
+    <tableColumn id="1" name="depth"/>
+    <tableColumn id="2" name="depth2"/>
+    <tableColumn id="3" name="depth3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1333,24 +1364,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F184B414-389F-4175-A968-082C604353C4}">
-  <dimension ref="B2:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1358,17 +1389,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1376,7 +1407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1384,12 +1415,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1397,12 +1428,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1410,17 +1441,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>17</v>
       </c>
@@ -1428,17 +1459,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>125</v>
       </c>
@@ -1446,14 +1477,19 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1467,20 +1503,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D3E8A5-FA88-49A3-9E2C-0F365D14ECC1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.3984375" customWidth="1"/>
-    <col min="2" max="2" width="28.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.4140625" customWidth="1"/>
+    <col min="2" max="2" width="28.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -1492,7 +1528,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1504,7 +1540,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1516,7 +1552,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1526,7 +1562,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1546,7 +1582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1556,7 +1592,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>52</v>
       </c>
@@ -1572,7 +1608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>53</v>
       </c>
@@ -1588,7 +1624,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="9"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1596,7 +1632,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1604,7 +1640,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="9"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1612,7 +1648,7 @@
       <c r="E14" s="11"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>34</v>
       </c>
@@ -1622,7 +1658,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1632,7 +1668,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1662,7 +1698,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="3"/>
@@ -1670,7 +1706,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -1686,7 +1722,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>48</v>
       </c>
@@ -1712,7 +1748,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1724,7 +1760,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1736,7 +1772,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +1814,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>30</v>
       </c>
@@ -1788,7 +1824,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>50</v>
       </c>
@@ -1854,7 +1890,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>37</v>
       </c>
@@ -1870,7 +1906,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>39</v>
       </c>
@@ -1896,7 +1932,7 @@
       <c r="E37" s="18"/>
       <c r="F37" s="19"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -1908,7 +1944,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -1920,12 +1956,12 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1962,7 +1998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>30</v>
       </c>
@@ -2022,7 +2058,7 @@
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>37</v>
       </c>
@@ -2038,7 +2074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>39</v>
       </c>
@@ -2064,7 +2100,7 @@
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="20" t="s">
         <v>41</v>
       </c>
@@ -2076,7 +2112,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>22</v>
       </c>
@@ -2088,7 +2124,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>23</v>
       </c>
@@ -2140,7 +2176,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>51</v>
       </c>
@@ -2156,7 +2192,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>53</v>
       </c>
@@ -2172,7 +2208,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="9" t="s">
         <v>56</v>
       </c>
@@ -2188,7 +2224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>57</v>
       </c>
@@ -2204,7 +2240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>59</v>
       </c>
@@ -2270,7 +2306,7 @@
       <c r="E68" s="15"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="9"/>
       <c r="B69" s="10"/>
       <c r="C69" s="3"/>
@@ -2278,7 +2314,7 @@
       <c r="E69" s="17"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>61</v>
       </c>
@@ -2294,7 +2330,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>37</v>
       </c>
@@ -2328,22 +2364,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D499F6F-363E-4019-B287-C75BA9D0ABD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F43" sqref="A24:F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="43.69921875" customWidth="1"/>
-    <col min="3" max="3" width="29.3984375" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.4140625" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -2355,7 +2391,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -2367,7 +2403,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2379,7 +2415,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -2389,7 +2425,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2409,7 +2445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -2419,7 +2455,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>71</v>
       </c>
@@ -2435,7 +2471,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -2445,7 +2481,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2455,7 +2491,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -2475,7 +2511,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -2485,7 +2521,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>76</v>
       </c>
@@ -2497,7 +2533,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -2507,7 +2543,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>75</v>
@@ -2521,7 +2557,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -2531,7 +2567,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="25" t="s">
         <v>68</v>
       </c>
@@ -2541,7 +2577,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -2549,7 +2585,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -2565,7 +2601,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
@@ -2581,7 +2617,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -2591,7 +2627,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -2603,7 +2639,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2615,7 +2651,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2627,7 +2663,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2637,7 +2673,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -2657,7 +2693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -2667,7 +2703,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>79</v>
       </c>
@@ -2733,7 +2769,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="10" t="s">
         <v>76</v>
       </c>
@@ -2745,7 +2781,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>30</v>
@@ -2755,7 +2791,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>75</v>
@@ -2769,7 +2805,7 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>34</v>
@@ -2779,7 +2815,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="25" t="s">
         <v>68</v>
       </c>
@@ -2789,7 +2825,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="3"/>
@@ -2797,7 +2833,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>37</v>
       </c>
@@ -2813,7 +2849,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
@@ -2846,23 +2882,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFED3AB1-87EB-4930-96AC-084E118F7317}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.19921875" customWidth="1"/>
-    <col min="3" max="3" width="33.796875" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -2874,7 +2910,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -2886,7 +2922,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2898,7 +2934,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -2908,7 +2944,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2928,7 +2964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -2938,7 +2974,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>76</v>
       </c>
@@ -2950,7 +2986,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>30</v>
@@ -2960,7 +2996,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>107</v>
@@ -2976,7 +3012,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>90</v>
@@ -2992,7 +3028,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>87</v>
@@ -3008,7 +3044,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>93</v>
@@ -3024,7 +3060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>95</v>
@@ -3040,7 +3076,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>96</v>
@@ -3056,7 +3092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>100</v>
@@ -3072,7 +3108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
         <v>105</v>
@@ -3088,7 +3124,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>101</v>
@@ -3104,7 +3140,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
         <v>99</v>
@@ -3120,7 +3156,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9"/>
       <c r="B19" s="10" t="s">
         <v>34</v>
@@ -3130,7 +3166,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="25" t="s">
         <v>68</v>
       </c>
@@ -3185,7 +3221,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>88</v>
       </c>
@@ -3201,7 +3237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
@@ -3227,7 +3263,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -3239,7 +3275,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -3251,7 +3287,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -3303,7 +3339,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="10" t="s">
         <v>76</v>
       </c>
@@ -3315,7 +3351,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>30</v>
@@ -3325,7 +3361,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>107</v>
@@ -3341,7 +3377,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>34</v>
@@ -3351,7 +3387,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="25" t="s">
         <v>68</v>
       </c>
@@ -3406,7 +3442,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>88</v>
       </c>
@@ -3422,7 +3458,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>39</v>
       </c>
@@ -3455,21 +3491,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E938BA-E7BA-4D35-9558-6B69D2DEE998}">
-  <dimension ref="A1:F102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="5" width="11.3984375" customWidth="1"/>
+    <col min="4" max="5" width="11.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -3481,7 +3517,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -3493,7 +3529,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -3505,7 +3541,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3515,7 +3551,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -3535,7 +3571,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3545,7 +3581,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>114</v>
       </c>
@@ -3561,7 +3597,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -3571,7 +3607,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3581,7 +3617,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -3601,7 +3637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -3611,7 +3647,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>76</v>
       </c>
@@ -3623,7 +3659,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -3633,7 +3669,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>75</v>
@@ -3647,7 +3683,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -3657,7 +3693,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="25" t="s">
         <v>68</v>
       </c>
@@ -3667,7 +3703,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -3675,7 +3711,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -3691,7 +3727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
@@ -3717,7 +3753,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3729,7 +3765,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -3741,7 +3777,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3793,7 +3829,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>114</v>
       </c>
@@ -3859,7 +3895,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>76</v>
       </c>
@@ -3871,7 +3907,7 @@
       <c r="E34" s="17"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
         <v>30</v>
@@ -3881,7 +3917,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>75</v>
@@ -3895,7 +3931,7 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>34</v>
@@ -3905,7 +3941,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="25" t="s">
         <v>68</v>
       </c>
@@ -3915,7 +3951,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="3"/>
@@ -3923,7 +3959,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>37</v>
       </c>
@@ -3939,7 +3975,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>39</v>
       </c>
@@ -3965,7 +4001,7 @@
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="20" t="s">
         <v>41</v>
       </c>
@@ -3977,7 +4013,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
@@ -3989,7 +4025,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -4041,7 +4077,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>53</v>
       </c>
@@ -4057,7 +4093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>56</v>
       </c>
@@ -4073,7 +4109,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>57</v>
       </c>
@@ -4089,7 +4125,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>59</v>
       </c>
@@ -4155,7 +4191,7 @@
       <c r="E58" s="15"/>
       <c r="F58" s="16"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="3"/>
@@ -4163,7 +4199,7 @@
       <c r="E59" s="17"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>118</v>
       </c>
@@ -4179,7 +4215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>37</v>
       </c>
@@ -4205,7 +4241,7 @@
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>21</v>
       </c>
@@ -4217,7 +4253,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>22</v>
       </c>
@@ -4229,7 +4265,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>23</v>
       </c>
@@ -4271,7 +4307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>30</v>
       </c>
@@ -4281,7 +4317,7 @@
       <c r="E70" s="11"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>50</v>
       </c>
@@ -4347,7 +4383,7 @@
       <c r="E75" s="15"/>
       <c r="F75" s="16"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="9" t="s">
         <v>37</v>
       </c>
@@ -4363,7 +4399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="9" t="s">
         <v>39</v>
       </c>
@@ -4389,7 +4425,7 @@
       <c r="E78" s="18"/>
       <c r="F78" s="19"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>21</v>
       </c>
@@ -4401,7 +4437,7 @@
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>22</v>
       </c>
@@ -4413,7 +4449,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>23</v>
       </c>
@@ -4465,7 +4501,7 @@
       <c r="E86" s="7"/>
       <c r="F86" s="8"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="9" t="s">
         <v>114</v>
       </c>
@@ -4531,7 +4567,7 @@
       <c r="E91" s="15"/>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="10" t="s">
         <v>76</v>
       </c>
@@ -4543,7 +4579,7 @@
       <c r="E92" s="17"/>
       <c r="F92" s="8"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="9"/>
       <c r="B93" s="10" t="s">
         <v>30</v>
@@ -4553,7 +4589,7 @@
       <c r="E93" s="17"/>
       <c r="F93" s="8"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
         <v>107</v>
@@ -4569,7 +4605,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
         <v>105</v>
@@ -4585,7 +4621,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="9"/>
       <c r="B96" s="10" t="s">
         <v>87</v>
@@ -4601,7 +4637,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="9"/>
       <c r="B97" s="10" t="s">
         <v>34</v>
@@ -4611,7 +4647,7 @@
       <c r="E97" s="17"/>
       <c r="F97" s="8"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="25" t="s">
         <v>68</v>
       </c>
@@ -4621,7 +4657,7 @@
       <c r="E98" s="17"/>
       <c r="F98" s="8"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="3"/>
@@ -4629,7 +4665,7 @@
       <c r="E99" s="17"/>
       <c r="F99" s="8"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="9" t="s">
         <v>37</v>
       </c>
@@ -4645,7 +4681,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="9" t="s">
         <v>39</v>
       </c>
@@ -4670,6 +4706,254 @@
       <c r="D102" s="14"/>
       <c r="E102" s="18"/>
       <c r="F102" s="19"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A105" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A106" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="8"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A110" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E110" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B111" s="13"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="8"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="16"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="8"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A116" s="9"/>
+      <c r="B116" s="10"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="8"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A117" s="9"/>
+      <c r="B117" s="10"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="8"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="9"/>
+      <c r="B118" s="10"/>
+      <c r="C118" s="30"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="17"/>
+      <c r="F118" s="8"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="9"/>
+      <c r="B119" s="10"/>
+      <c r="C119" s="30"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="8"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A120" s="9"/>
+      <c r="B120" s="10"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="8"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121" s="25"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="8"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A122" s="10"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="8"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E123" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B124" s="10"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E124" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="18"/>
+      <c r="F125" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4679,23 +4963,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C87D3C4-3CD4-4F17-875F-C2294F98A302}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.3984375" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" customWidth="1"/>
-    <col min="4" max="4" width="15.3984375" customWidth="1"/>
-    <col min="5" max="5" width="12.8984375" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="2" max="2" width="31.4140625" customWidth="1"/>
+    <col min="3" max="3" width="13.4140625" customWidth="1"/>
+    <col min="4" max="4" width="15.4140625" customWidth="1"/>
+    <col min="5" max="5" width="12.9140625" customWidth="1"/>
+    <col min="6" max="6" width="12.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
         <v>41</v>
       </c>
@@ -4707,7 +4991,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -4719,7 +5003,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -4731,7 +5015,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -4741,7 +5025,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -4761,7 +5045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4771,7 +5055,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>130</v>
       </c>
@@ -4787,7 +5071,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>132</v>
       </c>
@@ -4803,7 +5087,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>141</v>
       </c>
@@ -4819,7 +5103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="9"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4827,7 +5111,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -4835,7 +5119,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
@@ -4845,7 +5129,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -4855,7 +5139,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -4875,7 +5159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -4885,7 +5169,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>139</v>
       </c>
@@ -4901,7 +5185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>47</v>
       </c>
@@ -4917,7 +5201,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>62</v>
       </c>
@@ -4933,7 +5217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
@@ -4943,7 +5227,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -4953,7 +5237,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>41</v>
       </c>
@@ -4965,7 +5249,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -4977,19 +5261,19 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -4999,7 +5283,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -5019,7 +5303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -5029,7 +5313,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>141</v>
       </c>
@@ -5045,7 +5329,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="9"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5053,7 +5337,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="9"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5061,7 +5345,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="9"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5069,7 +5353,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="9"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5077,7 +5361,7 @@
       <c r="E33" s="11"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>34</v>
       </c>
@@ -5087,7 +5371,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -5097,7 +5381,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
@@ -5117,7 +5401,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>30</v>
       </c>
@@ -5127,7 +5411,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>139</v>
       </c>
@@ -5143,7 +5427,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>47</v>
       </c>
@@ -5159,7 +5443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="3"/>
@@ -5167,7 +5451,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>34</v>
       </c>
@@ -5177,7 +5461,7 @@
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>41</v>
       </c>
@@ -5189,7 +5473,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -5201,19 +5485,19 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -5223,7 +5507,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>26</v>
       </c>
@@ -5243,7 +5527,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>30</v>
       </c>
@@ -5253,7 +5537,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>130</v>
       </c>
@@ -5269,7 +5553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>132</v>
       </c>
@@ -5285,7 +5569,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="9"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5293,7 +5577,7 @@
       <c r="E51" s="11"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="9"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5301,7 +5585,7 @@
       <c r="E52" s="11"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="9"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5359,7 +5643,7 @@
       <c r="E57" s="15"/>
       <c r="F57" s="16"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>139</v>
       </c>
@@ -5375,7 +5659,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>47</v>
       </c>
@@ -5391,7 +5675,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="3"/>
@@ -5412,5 +5696,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[docs] API 문서 수정
</commit_message>
<xml_diff>
--- a/docs/API.xlsx
+++ b/docs/API.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Property\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\Property\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="810" windowWidth="23260" windowHeight="12580" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="1500" windowWidth="23265" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="메인" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="159">
   <si>
     <t>api 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -741,10 +741,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DELETE</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -770,6 +766,22 @@
   </si>
   <si>
     <t>ethaccount: ""</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래완료된목록을 컨트랙트에서 db로 쏴줘야 거래이루어졌던 목록을 보여줄수있다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결국백에서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로고침을 하게하던지, 새로고침 해야 업데이트되게하던지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1365,23 +1377,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D21"/>
+  <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1389,17 +1401,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1407,7 +1419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1415,12 +1427,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1428,12 +1440,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1441,17 +1453,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>17</v>
       </c>
@@ -1459,17 +1471,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>125</v>
       </c>
@@ -1477,19 +1489,37 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>151</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1506,17 +1536,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.4140625" customWidth="1"/>
-    <col min="2" max="2" width="28.4140625" customWidth="1"/>
+    <col min="1" max="1" width="31.375" customWidth="1"/>
+    <col min="2" max="2" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -1528,7 +1558,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1540,7 +1570,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1552,7 +1582,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1562,7 +1592,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1582,7 +1612,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1592,7 +1622,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>52</v>
       </c>
@@ -1608,7 +1638,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>53</v>
       </c>
@@ -1624,7 +1654,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1632,7 +1662,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1640,7 +1670,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1648,7 +1678,7 @@
       <c r="E14" s="11"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>34</v>
       </c>
@@ -1658,7 +1688,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1668,7 +1698,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1688,7 +1718,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
@@ -1698,7 +1728,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="3"/>
@@ -1706,7 +1736,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -1722,7 +1752,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>48</v>
       </c>
@@ -1738,7 +1768,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>34</v>
       </c>
@@ -1748,7 +1778,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1760,7 +1790,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1802,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1784,7 +1814,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1794,7 +1824,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -1814,7 +1844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>30</v>
       </c>
@@ -1824,7 +1854,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>50</v>
       </c>
@@ -1840,7 +1870,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>34</v>
       </c>
@@ -1850,7 +1880,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1860,7 +1890,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -1880,7 +1910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
@@ -1890,7 +1920,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>37</v>
       </c>
@@ -1906,7 +1936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>39</v>
       </c>
@@ -1922,7 +1952,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>34</v>
       </c>
@@ -1932,7 +1962,7 @@
       <c r="E37" s="18"/>
       <c r="F37" s="19"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -1944,7 +1974,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
@@ -1956,19 +1986,19 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1978,7 +2008,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>26</v>
       </c>
@@ -1998,7 +2028,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>30</v>
       </c>
@@ -2008,7 +2038,7 @@
       <c r="E45" s="11"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>34</v>
       </c>
@@ -2018,7 +2048,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
@@ -2028,7 +2058,7 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>26</v>
       </c>
@@ -2048,7 +2078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>30</v>
       </c>
@@ -2058,7 +2088,7 @@
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>37</v>
       </c>
@@ -2074,7 +2104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>39</v>
       </c>
@@ -2090,7 +2120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>34</v>
       </c>
@@ -2100,7 +2130,7 @@
       <c r="E52" s="18"/>
       <c r="F52" s="19"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
         <v>41</v>
       </c>
@@ -2112,7 +2142,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>22</v>
       </c>
@@ -2124,7 +2154,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>23</v>
       </c>
@@ -2136,7 +2166,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>25</v>
       </c>
@@ -2146,7 +2176,7 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>26</v>
       </c>
@@ -2166,7 +2196,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>30</v>
       </c>
@@ -2176,7 +2206,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>51</v>
       </c>
@@ -2192,7 +2222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>53</v>
       </c>
@@ -2208,7 +2238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>56</v>
       </c>
@@ -2224,7 +2254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>57</v>
       </c>
@@ -2240,7 +2270,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>59</v>
       </c>
@@ -2256,7 +2286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>34</v>
       </c>
@@ -2266,7 +2296,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="17"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>35</v>
       </c>
@@ -2276,7 +2306,7 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>26</v>
       </c>
@@ -2296,7 +2326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>30</v>
       </c>
@@ -2306,7 +2336,7 @@
       <c r="E68" s="15"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="10"/>
       <c r="C69" s="3"/>
@@ -2314,7 +2344,7 @@
       <c r="E69" s="17"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>61</v>
       </c>
@@ -2330,7 +2360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>37</v>
       </c>
@@ -2346,7 +2376,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="s">
         <v>34</v>
       </c>
@@ -2371,15 +2401,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.4140625" customWidth="1"/>
-    <col min="5" max="5" width="13.08203125" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="3" max="3" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -2391,7 +2421,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2433,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2415,7 +2445,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -2425,7 +2455,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2475,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -2455,7 +2485,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>71</v>
       </c>
@@ -2471,7 +2501,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -2481,7 +2511,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2491,7 +2521,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -2511,7 +2541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -2521,7 +2551,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>76</v>
       </c>
@@ -2533,7 +2563,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -2543,7 +2573,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>75</v>
@@ -2557,7 +2587,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -2567,7 +2597,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>68</v>
       </c>
@@ -2577,7 +2607,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -2585,7 +2615,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -2601,7 +2631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
@@ -2617,7 +2647,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -2627,7 +2657,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -2639,7 +2669,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2651,7 +2681,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2663,7 +2693,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2673,7 +2703,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -2693,7 +2723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -2703,7 +2733,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>79</v>
       </c>
@@ -2719,7 +2749,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>34</v>
       </c>
@@ -2729,7 +2759,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -2739,7 +2769,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -2759,7 +2789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
@@ -2769,7 +2799,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>76</v>
       </c>
@@ -2781,7 +2811,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>30</v>
@@ -2791,7 +2821,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>75</v>
@@ -2805,7 +2835,7 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>34</v>
@@ -2815,7 +2845,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>68</v>
       </c>
@@ -2825,7 +2855,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="3"/>
@@ -2833,7 +2863,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>37</v>
       </c>
@@ -2849,7 +2879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
@@ -2865,7 +2895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>34</v>
       </c>
@@ -2889,16 +2919,16 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="33.875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.4140625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -2910,7 +2940,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -2922,7 +2952,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2934,7 +2964,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -2944,7 +2974,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -2964,7 +2994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -2974,7 +3004,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>76</v>
       </c>
@@ -2986,7 +3016,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>30</v>
@@ -2996,7 +3026,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>107</v>
@@ -3012,7 +3042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>90</v>
@@ -3028,7 +3058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>87</v>
@@ -3044,7 +3074,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>93</v>
@@ -3060,7 +3090,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>95</v>
@@ -3076,7 +3106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>96</v>
@@ -3092,7 +3122,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>100</v>
@@ -3108,7 +3138,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
         <v>105</v>
@@ -3124,7 +3154,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>101</v>
@@ -3140,7 +3170,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
         <v>99</v>
@@ -3156,7 +3186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="10" t="s">
         <v>34</v>
@@ -3166,7 +3196,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>68</v>
       </c>
@@ -3176,7 +3206,7 @@
       <c r="E20" s="17"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>34</v>
       </c>
@@ -3186,7 +3216,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>86</v>
       </c>
@@ -3196,7 +3226,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -3216,12 +3246,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>88</v>
       </c>
@@ -3237,7 +3267,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
@@ -3253,7 +3283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>34</v>
       </c>
@@ -3263,7 +3293,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -3275,7 +3305,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -3287,7 +3317,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -3299,7 +3329,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
@@ -3309,7 +3339,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -3329,7 +3359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
@@ -3339,7 +3369,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>76</v>
       </c>
@@ -3351,7 +3381,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>30</v>
@@ -3361,7 +3391,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>107</v>
@@ -3377,7 +3407,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>34</v>
@@ -3387,7 +3417,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>68</v>
       </c>
@@ -3397,7 +3427,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>34</v>
       </c>
@@ -3407,7 +3437,7 @@
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>86</v>
       </c>
@@ -3417,7 +3447,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>26</v>
       </c>
@@ -3437,12 +3467,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>88</v>
       </c>
@@ -3458,7 +3488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>39</v>
       </c>
@@ -3474,7 +3504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>34</v>
       </c>
@@ -3494,18 +3524,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="5" width="11.4140625" customWidth="1"/>
+    <col min="4" max="5" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -3517,7 +3547,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -3529,7 +3559,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -3541,7 +3571,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3551,7 +3581,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -3571,7 +3601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3581,7 +3611,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>114</v>
       </c>
@@ -3597,7 +3627,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -3607,7 +3637,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3617,7 +3647,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -3637,7 +3667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -3647,7 +3677,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>76</v>
       </c>
@@ -3659,7 +3689,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -3669,7 +3699,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>75</v>
@@ -3683,7 +3713,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -3693,7 +3723,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>68</v>
       </c>
@@ -3703,7 +3733,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -3711,7 +3741,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -3727,7 +3757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
@@ -3743,7 +3773,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -3753,7 +3783,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3765,7 +3795,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -3777,7 +3807,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3789,7 +3819,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -3799,7 +3829,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -3819,7 +3849,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -3829,7 +3859,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>114</v>
       </c>
@@ -3845,7 +3875,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
@@ -3855,7 +3885,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -3865,7 +3895,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>26</v>
       </c>
@@ -3885,7 +3915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
@@ -3895,7 +3925,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>76</v>
       </c>
@@ -3907,7 +3937,7 @@
       <c r="E34" s="17"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
         <v>30</v>
@@ -3917,7 +3947,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>75</v>
@@ -3931,7 +3961,7 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>34</v>
@@ -3941,7 +3971,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>68</v>
       </c>
@@ -3951,7 +3981,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="3"/>
@@ -3959,7 +3989,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>37</v>
       </c>
@@ -3975,7 +4005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>39</v>
       </c>
@@ -3991,7 +4021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>34</v>
       </c>
@@ -4001,7 +4031,7 @@
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
         <v>41</v>
       </c>
@@ -4013,7 +4043,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
@@ -4025,7 +4055,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -4037,7 +4067,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -4047,7 +4077,7 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>26</v>
       </c>
@@ -4067,7 +4097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>30</v>
       </c>
@@ -4077,7 +4107,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>53</v>
       </c>
@@ -4093,7 +4123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>56</v>
       </c>
@@ -4109,7 +4139,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>57</v>
       </c>
@@ -4125,7 +4155,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>59</v>
       </c>
@@ -4141,7 +4171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>34</v>
       </c>
@@ -4151,7 +4181,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="17"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
@@ -4161,7 +4191,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>26</v>
       </c>
@@ -4181,7 +4211,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -4191,7 +4221,7 @@
       <c r="E58" s="15"/>
       <c r="F58" s="16"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="3"/>
@@ -4199,7 +4229,7 @@
       <c r="E59" s="17"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>118</v>
       </c>
@@ -4215,7 +4245,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>37</v>
       </c>
@@ -4231,7 +4261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>34</v>
       </c>
@@ -4241,7 +4271,7 @@
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>21</v>
       </c>
@@ -4253,7 +4283,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>22</v>
       </c>
@@ -4265,7 +4295,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>23</v>
       </c>
@@ -4277,7 +4307,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
@@ -4287,7 +4317,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>26</v>
       </c>
@@ -4307,7 +4337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>30</v>
       </c>
@@ -4317,7 +4347,7 @@
       <c r="E70" s="11"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>50</v>
       </c>
@@ -4333,7 +4363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="s">
         <v>34</v>
       </c>
@@ -4343,7 +4373,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>35</v>
       </c>
@@ -4353,7 +4383,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
@@ -4373,7 +4403,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>30</v>
       </c>
@@ -4383,7 +4413,7 @@
       <c r="E75" s="15"/>
       <c r="F75" s="16"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>37</v>
       </c>
@@ -4399,7 +4429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>39</v>
       </c>
@@ -4415,7 +4445,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
         <v>34</v>
       </c>
@@ -4425,7 +4455,7 @@
       <c r="E78" s="18"/>
       <c r="F78" s="19"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>21</v>
       </c>
@@ -4437,7 +4467,7 @@
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>22</v>
       </c>
@@ -4449,7 +4479,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>23</v>
       </c>
@@ -4461,7 +4491,7 @@
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>25</v>
       </c>
@@ -4471,7 +4501,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>26</v>
       </c>
@@ -4491,7 +4521,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>30</v>
       </c>
@@ -4501,7 +4531,7 @@
       <c r="E86" s="7"/>
       <c r="F86" s="8"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>114</v>
       </c>
@@ -4517,7 +4547,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="s">
         <v>34</v>
       </c>
@@ -4527,7 +4557,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="8"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>35</v>
       </c>
@@ -4537,7 +4567,7 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>26</v>
       </c>
@@ -4557,7 +4587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>30</v>
       </c>
@@ -4567,7 +4597,7 @@
       <c r="E91" s="15"/>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>76</v>
       </c>
@@ -4579,7 +4609,7 @@
       <c r="E92" s="17"/>
       <c r="F92" s="8"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
       <c r="B93" s="10" t="s">
         <v>30</v>
@@ -4589,7 +4619,7 @@
       <c r="E93" s="17"/>
       <c r="F93" s="8"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
         <v>107</v>
@@ -4605,7 +4635,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
         <v>105</v>
@@ -4621,7 +4651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="9"/>
       <c r="B96" s="10" t="s">
         <v>87</v>
@@ -4637,7 +4667,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="9"/>
       <c r="B97" s="10" t="s">
         <v>34</v>
@@ -4647,7 +4677,7 @@
       <c r="E97" s="17"/>
       <c r="F97" s="8"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="25" t="s">
         <v>68</v>
       </c>
@@ -4657,7 +4687,7 @@
       <c r="E98" s="17"/>
       <c r="F98" s="8"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="3"/>
@@ -4665,7 +4695,7 @@
       <c r="E99" s="17"/>
       <c r="F99" s="8"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
         <v>37</v>
       </c>
@@ -4681,7 +4711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
         <v>39</v>
       </c>
@@ -4697,7 +4727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="s">
         <v>34</v>
       </c>
@@ -4707,31 +4737,31 @@
       <c r="E102" s="18"/>
       <c r="F102" s="19"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>23</v>
       </c>
@@ -4743,7 +4773,7 @@
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>25</v>
       </c>
@@ -4753,7 +4783,7 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>26</v>
       </c>
@@ -4773,7 +4803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>30</v>
       </c>
@@ -4783,14 +4813,14 @@
       <c r="E109" s="7"/>
       <c r="F109" s="8"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E110" s="23" t="s">
         <v>92</v>
@@ -4799,7 +4829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>34</v>
       </c>
@@ -4809,7 +4839,7 @@
       <c r="E111" s="14"/>
       <c r="F111" s="8"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>35</v>
       </c>
@@ -4819,7 +4849,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>26</v>
       </c>
@@ -4839,7 +4869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>30</v>
       </c>
@@ -4849,7 +4879,7 @@
       <c r="E114" s="15"/>
       <c r="F114" s="16"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="3"/>
@@ -4857,7 +4887,7 @@
       <c r="E115" s="17"/>
       <c r="F115" s="8"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="9"/>
       <c r="B116" s="10"/>
       <c r="C116" s="3"/>
@@ -4865,7 +4895,7 @@
       <c r="E116" s="17"/>
       <c r="F116" s="8"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="9"/>
       <c r="B117" s="10"/>
       <c r="C117" s="3"/>
@@ -4873,7 +4903,7 @@
       <c r="E117" s="17"/>
       <c r="F117" s="8"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="9"/>
       <c r="B118" s="10"/>
       <c r="C118" s="30"/>
@@ -4881,7 +4911,7 @@
       <c r="E118" s="17"/>
       <c r="F118" s="8"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="9"/>
       <c r="B119" s="10"/>
       <c r="C119" s="30"/>
@@ -4889,7 +4919,7 @@
       <c r="E119" s="24"/>
       <c r="F119" s="8"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="9"/>
       <c r="B120" s="10"/>
       <c r="C120" s="3"/>
@@ -4897,7 +4927,7 @@
       <c r="E120" s="17"/>
       <c r="F120" s="8"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="25"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -4905,7 +4935,7 @@
       <c r="E121" s="17"/>
       <c r="F121" s="8"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
       <c r="C122" s="3"/>
@@ -4913,7 +4943,7 @@
       <c r="E122" s="17"/>
       <c r="F122" s="8"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="9" t="s">
         <v>37</v>
       </c>
@@ -4929,7 +4959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="9" t="s">
         <v>39</v>
       </c>
@@ -4945,7 +4975,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
         <v>34</v>
       </c>
@@ -4970,16 +5000,16 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.4140625" customWidth="1"/>
-    <col min="3" max="3" width="13.4140625" customWidth="1"/>
-    <col min="4" max="4" width="15.4140625" customWidth="1"/>
-    <col min="5" max="5" width="12.9140625" customWidth="1"/>
-    <col min="6" max="6" width="12.4140625" customWidth="1"/>
+    <col min="2" max="2" width="31.375" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>41</v>
       </c>
@@ -4991,7 +5021,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -5003,7 +5033,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -5015,7 +5045,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -5025,7 +5055,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -5045,7 +5075,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -5055,7 +5085,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>130</v>
       </c>
@@ -5071,7 +5101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>132</v>
       </c>
@@ -5087,7 +5117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>141</v>
       </c>
@@ -5103,7 +5133,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5111,7 +5141,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5119,7 +5149,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
@@ -5129,7 +5159,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -5139,7 +5169,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -5159,7 +5189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -5169,7 +5199,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>139</v>
       </c>
@@ -5185,7 +5215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>47</v>
       </c>
@@ -5201,7 +5231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>62</v>
       </c>
@@ -5217,7 +5247,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
@@ -5227,7 +5257,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -5237,7 +5267,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>41</v>
       </c>
@@ -5249,7 +5279,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -5261,19 +5291,19 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -5283,7 +5313,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -5303,7 +5333,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -5313,7 +5343,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>141</v>
       </c>
@@ -5329,7 +5359,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5337,7 +5367,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5345,7 +5375,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5353,7 +5383,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5361,7 +5391,7 @@
       <c r="E33" s="11"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>34</v>
       </c>
@@ -5371,7 +5401,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -5381,7 +5411,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
@@ -5401,7 +5431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>30</v>
       </c>
@@ -5411,7 +5441,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>139</v>
       </c>
@@ -5427,7 +5457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>47</v>
       </c>
@@ -5443,7 +5473,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="3"/>
@@ -5451,7 +5481,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>34</v>
       </c>
@@ -5461,7 +5491,7 @@
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>41</v>
       </c>
@@ -5473,7 +5503,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -5485,19 +5515,19 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -5507,7 +5537,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>26</v>
       </c>
@@ -5527,7 +5557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>30</v>
       </c>
@@ -5537,7 +5567,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>130</v>
       </c>
@@ -5553,7 +5583,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>132</v>
       </c>
@@ -5569,7 +5599,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5577,7 +5607,7 @@
       <c r="E51" s="11"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5585,7 +5615,7 @@
       <c r="E52" s="11"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -5593,7 +5623,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>34</v>
       </c>
@@ -5603,7 +5633,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="17"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
@@ -5613,7 +5643,7 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>26</v>
       </c>
@@ -5633,7 +5663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>30</v>
       </c>
@@ -5643,7 +5673,7 @@
       <c r="E57" s="15"/>
       <c r="F57" s="16"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
         <v>139</v>
       </c>
@@ -5659,7 +5689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>47</v>
       </c>
@@ -5675,7 +5705,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="3"/>
@@ -5683,7 +5713,7 @@
       <c r="E60" s="17"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
[docs] 12.25 API 수정
</commit_message>
<xml_diff>
--- a/docs/API.xlsx
+++ b/docs/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1500" windowWidth="23265" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="2190" windowWidth="23265" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="메인" sheetId="1" r:id="rId1"/>
@@ -789,9 +789,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1010,7 +1011,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1052,6 +1053,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1377,14 +1381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D27"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1520,6 +1525,11 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="31">
+        <v>43824</v>
       </c>
     </row>
   </sheetData>
@@ -1536,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[docs] 26일 02:26 API 수정
</commit_message>
<xml_diff>
--- a/docs/API.xlsx
+++ b/docs/API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="2880" windowWidth="23265" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="3570" windowWidth="23265" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="메인" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="187">
   <si>
     <t>api 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -387,10 +387,6 @@
     <t>],</t>
   </si>
   <si>
-    <t>home/popularList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>인기있는 방목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -423,10 +419,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>home/recentList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -494,27 +486,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"option":"",</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>옵션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>true,false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"imgPath": ""</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"roomSize","",</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"roomCount","",</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -808,6 +780,229 @@
     <t>로그인 버튼</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/popularList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/recentList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물찾기 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물등록 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/properties-register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/properties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>관여</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roomFloor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roomPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"roomSize":"",</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"roomCount":"",</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"roomType": "",</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물형태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>html name들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roomArea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rootType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{ DB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>컬럼</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roomNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imgPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"owner_id":"",</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>관여</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>임대인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_number</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -818,7 +1013,7 @@
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,6 +1062,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1408,7 +1610,7 @@
   <dimension ref="A2:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1512,43 +1714,43 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1570,7 +1772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1597,7 +1799,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1609,7 +1811,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1817,7 +2019,7 @@
         <v>41</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1829,7 +2031,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2061,7 +2263,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2257,7 +2459,7 @@
         <v>23</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2401,7 +2603,7 @@
         <v>41</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2425,7 +2627,7 @@
         <v>23</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -2657,7 +2859,7 @@
         <v>41</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -2669,7 +2871,7 @@
         <v>22</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
@@ -2917,10 +3119,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2936,7 +3138,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2948,7 +3150,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3009,18 +3211,18 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="F7" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3075,7 +3277,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="3"/>
@@ -3098,7 +3300,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="11" t="s">
@@ -3184,7 +3386,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -3196,7 +3398,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>160</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -3257,18 +3459,18 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -3323,7 +3525,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="3"/>
@@ -3346,7 +3548,7 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="11" t="s">
@@ -3427,9 +3629,506 @@
       <c r="E43" s="18"/>
       <c r="F43" s="19"/>
     </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="16"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="17"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="19"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="16"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="9"/>
+      <c r="B80" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="9"/>
+      <c r="B81" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E81" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="9"/>
+      <c r="B82" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C82" s="3"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="10"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="10"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="19"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3437,8 +4136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3455,7 +4154,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3467,7 +4166,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3488,7 +4187,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3526,14 +4225,13 @@
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="3"/>
       <c r="D7" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="8"/>
@@ -3541,88 +4239,100 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="D8" s="11"/>
       <c r="E8" s="17"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>166</v>
+      </c>
       <c r="D9" s="11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="30"/>
+        <v>183</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>184</v>
+      </c>
       <c r="D10" s="11" t="s">
-        <v>90</v>
+        <v>185</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>91</v>
+        <v>186</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="30"/>
+        <v>87</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>165</v>
+      </c>
       <c r="D11" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="24" t="s">
         <v>88</v>
       </c>
+      <c r="E11" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="F11" s="8" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>166</v>
+      </c>
       <c r="D12" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>91</v>
+        <v>65</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="30"/>
+        <v>90</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="D13" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>72</v>
+        <v>91</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>89</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>33</v>
@@ -3631,14 +4341,16 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="30"/>
+        <v>92</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>168</v>
+      </c>
       <c r="D14" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>33</v>
@@ -3647,57 +4359,65 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="11" t="s">
-        <v>102</v>
+        <v>171</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="30"/>
+        <v>169</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>175</v>
+      </c>
       <c r="D16" s="11" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="30"/>
+        <v>170</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>178</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E17" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="30"/>
+        <v>93</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>179</v>
+      </c>
       <c r="D18" s="11" t="s">
         <v>66</v>
       </c>
@@ -3740,7 +4460,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3770,12 +4490,12 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="3"/>
@@ -3820,7 +4540,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -3832,7 +4552,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -3844,7 +4564,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3853,7 +4573,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3893,12 +4613,12 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="3"/>
       <c r="D35" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
@@ -3916,17 +4636,17 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E37" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3961,7 +4681,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3991,12 +4711,12 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="3"/>
@@ -4046,7 +4766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
@@ -4062,7 +4782,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4074,7 +4794,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4086,7 +4806,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4135,18 +4855,18 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="26" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -4201,7 +4921,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="3"/>
@@ -4224,7 +4944,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="11" t="s">
@@ -4310,7 +5030,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -4322,7 +5042,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4383,18 +5103,18 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="26" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4449,7 +5169,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="3"/>
@@ -4472,7 +5192,7 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="11" t="s">
@@ -4558,7 +5278,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -4570,7 +5290,7 @@
         <v>22</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -4582,7 +5302,7 @@
         <v>23</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -4753,7 +5473,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3"/>
@@ -4798,7 +5518,7 @@
         <v>21</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -4810,7 +5530,7 @@
         <v>22</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -4822,7 +5542,7 @@
         <v>23</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -4982,7 +5702,7 @@
         <v>21</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -4994,7 +5714,7 @@
         <v>22</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -5055,18 +5775,18 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="26" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E87" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -5121,7 +5841,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="3"/>
@@ -5144,49 +5864,49 @@
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E94" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F94" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C95" s="30"/>
       <c r="D95" s="11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="9"/>
       <c r="B96" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C96" s="30"/>
       <c r="D96" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E96" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -5264,7 +5984,7 @@
         <v>21</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
@@ -5276,7 +5996,7 @@
         <v>22</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
@@ -5337,18 +6057,18 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="26" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E110" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -5536,7 +6256,7 @@
         <v>41</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5548,7 +6268,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5609,12 +6329,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="26" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>44</v>
@@ -5625,15 +6345,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="22" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>33</v>
@@ -5641,18 +6361,18 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="22" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5723,7 +6443,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="3"/>
@@ -5731,7 +6451,7 @@
         <v>46</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>33</v>
@@ -5744,7 +6464,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="26" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>32</v>
@@ -5760,7 +6480,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="3"/>
       <c r="D18" s="22" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>62</v>
@@ -5794,7 +6514,7 @@
         <v>41</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -5806,7 +6526,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -5818,7 +6538,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -5867,18 +6587,18 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="22" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E29" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -5965,7 +6685,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="3"/>
@@ -5973,7 +6693,7 @@
         <v>46</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>33</v>
@@ -5986,7 +6706,7 @@
       <c r="B39" s="10"/>
       <c r="C39" s="3"/>
       <c r="D39" s="26" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>32</v>
@@ -6018,7 +6738,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -6030,7 +6750,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -6042,7 +6762,7 @@
         <v>23</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -6091,12 +6811,12 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="3"/>
       <c r="D49" s="26" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>44</v>
@@ -6107,15 +6827,15 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="22" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>33</v>
@@ -6197,7 +6917,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="3"/>
@@ -6205,7 +6925,7 @@
         <v>46</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>33</v>
@@ -6218,7 +6938,7 @@
       <c r="B59" s="10"/>
       <c r="C59" s="3"/>
       <c r="D59" s="26" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
[docs] 12.29 19:47 API 수정
</commit_message>
<xml_diff>
--- a/docs/API.xlsx
+++ b/docs/API.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\Property\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Property\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="3570" windowWidth="23265" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="4030" windowWidth="23270" windowHeight="12590" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="메인" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="189">
   <si>
     <t>api 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,10 +430,6 @@
     <t>목록</t>
   </si>
   <si>
-    <t>/roomRegister</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>매물 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -551,10 +547,6 @@
   </si>
   <si>
     <t>찜목록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>myPage/wishList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1001,6 +993,22 @@
   </si>
   <si>
     <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 후 로그인페이지 로드</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/register/signin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/properties-register/roomRegister</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>myWishList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1613,18 +1621,18 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1632,17 +1640,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1650,7 +1658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1658,12 +1666,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1671,12 +1679,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1684,17 +1692,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>17</v>
       </c>
@@ -1702,58 +1710,58 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
         <v>117</v>
       </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="31">
         <v>43824</v>
       </c>
@@ -1770,19 +1778,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F111"/>
+  <dimension ref="A2:F131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.375" customWidth="1"/>
-    <col min="2" max="2" width="28.375" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="20" t="s">
         <v>41</v>
       </c>
@@ -1794,31 +1802,31 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1828,7 +1836,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1858,7 +1866,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>52</v>
       </c>
@@ -1874,7 +1882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>53</v>
       </c>
@@ -1890,7 +1898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="9"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1898,7 +1906,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1906,7 +1914,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="9"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1914,7 +1922,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>34</v>
       </c>
@@ -1924,7 +1932,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1934,7 +1942,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1954,7 +1962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -1964,7 +1972,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -1972,7 +1980,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
@@ -1988,7 +1996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>48</v>
       </c>
@@ -2004,7 +2012,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -2014,31 +2022,31 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2050,7 +2058,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2060,7 +2068,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -2080,7 +2088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -2090,7 +2098,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>52</v>
       </c>
@@ -2106,7 +2114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>53</v>
       </c>
@@ -2122,7 +2130,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="9"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2130,7 +2138,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="9"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2138,7 +2146,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="9"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2146,7 +2154,7 @@
       <c r="E33" s="11"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>34</v>
       </c>
@@ -2156,7 +2164,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -2166,7 +2174,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
@@ -2186,7 +2194,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>30</v>
       </c>
@@ -2196,7 +2204,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="3"/>
@@ -2204,7 +2212,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>47</v>
       </c>
@@ -2220,7 +2228,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>48</v>
       </c>
@@ -2236,7 +2244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>34</v>
       </c>
@@ -2246,7 +2254,7 @@
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
@@ -2258,19 +2266,19 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -2282,7 +2290,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -2292,7 +2300,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>26</v>
       </c>
@@ -2312,7 +2320,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>30</v>
       </c>
@@ -2322,7 +2330,7 @@
       <c r="E48" s="11"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>50</v>
       </c>
@@ -2338,7 +2346,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>34</v>
       </c>
@@ -2348,7 +2356,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
@@ -2358,7 +2366,7 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>26</v>
       </c>
@@ -2378,7 +2386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>30</v>
       </c>
@@ -2388,7 +2396,7 @@
       <c r="E53" s="15"/>
       <c r="F53" s="16"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>37</v>
       </c>
@@ -2404,7 +2412,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>39</v>
       </c>
@@ -2420,7 +2428,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>34</v>
       </c>
@@ -2430,7 +2438,7 @@
       <c r="E56" s="18"/>
       <c r="F56" s="19"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>21</v>
       </c>
@@ -2442,7 +2450,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>22</v>
       </c>
@@ -2454,19 +2462,19 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
@@ -2476,7 +2484,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>26</v>
       </c>
@@ -2496,7 +2504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>30</v>
       </c>
@@ -2506,7 +2514,7 @@
       <c r="E64" s="11"/>
       <c r="F64" s="8"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>34</v>
       </c>
@@ -2516,7 +2524,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="8"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>35</v>
       </c>
@@ -2526,7 +2534,7 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>26</v>
       </c>
@@ -2546,7 +2554,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>30</v>
       </c>
@@ -2556,7 +2564,7 @@
       <c r="E68" s="15"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="9" t="s">
         <v>37</v>
       </c>
@@ -2572,7 +2580,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>39</v>
       </c>
@@ -2588,7 +2596,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>34</v>
       </c>
@@ -2598,19 +2606,19 @@
       <c r="E71" s="18"/>
       <c r="F71" s="19"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>22</v>
       </c>
@@ -2622,19 +2630,19 @@
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>25</v>
       </c>
@@ -2644,7 +2652,7 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>26</v>
       </c>
@@ -2664,7 +2672,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>30</v>
       </c>
@@ -2674,7 +2682,7 @@
       <c r="E78" s="7"/>
       <c r="F78" s="17"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="9" t="s">
         <v>51</v>
       </c>
@@ -2690,7 +2698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="9" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="9" t="s">
         <v>55</v>
       </c>
@@ -2722,7 +2730,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="9" t="s">
         <v>56</v>
       </c>
@@ -2738,7 +2746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="9" t="s">
         <v>58</v>
       </c>
@@ -2754,7 +2762,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>34</v>
       </c>
@@ -2764,7 +2772,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>35</v>
       </c>
@@ -2774,7 +2782,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>30</v>
       </c>
@@ -2804,7 +2812,7 @@
       <c r="E87" s="15"/>
       <c r="F87" s="16"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="9"/>
       <c r="B88" s="10"/>
       <c r="C88" s="3"/>
@@ -2812,7 +2820,7 @@
       <c r="E88" s="17"/>
       <c r="F88" s="8"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="9" t="s">
         <v>60</v>
       </c>
@@ -2828,7 +2836,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="9" t="s">
         <v>37</v>
       </c>
@@ -2844,7 +2852,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>34</v>
       </c>
@@ -2854,31 +2862,31 @@
       <c r="E91" s="18"/>
       <c r="F91" s="19"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>23</v>
       </c>
@@ -2890,7 +2898,7 @@
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>25</v>
       </c>
@@ -2900,7 +2908,7 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>26</v>
       </c>
@@ -2920,7 +2928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>30</v>
       </c>
@@ -2930,7 +2938,7 @@
       <c r="E98" s="7"/>
       <c r="F98" s="17"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="9" t="s">
         <v>51</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="9" t="s">
         <v>53</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="9" t="s">
         <v>55</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="9" t="s">
         <v>56</v>
       </c>
@@ -2994,7 +3002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="9" t="s">
         <v>58</v>
       </c>
@@ -3010,7 +3018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>34</v>
       </c>
@@ -3020,7 +3028,7 @@
       <c r="E104" s="14"/>
       <c r="F104" s="17"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>35</v>
       </c>
@@ -3030,7 +3038,7 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>26</v>
       </c>
@@ -3050,7 +3058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>30</v>
       </c>
@@ -3060,7 +3068,7 @@
       <c r="E107" s="15"/>
       <c r="F107" s="16"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="9"/>
       <c r="B108" s="10"/>
       <c r="C108" s="3"/>
@@ -3068,7 +3076,7 @@
       <c r="E108" s="17"/>
       <c r="F108" s="8"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="9" t="s">
         <v>60</v>
       </c>
@@ -3084,7 +3092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="9" t="s">
         <v>37</v>
       </c>
@@ -3100,7 +3108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>34</v>
       </c>
@@ -3109,6 +3117,206 @@
       <c r="D111" s="14"/>
       <c r="E111" s="18"/>
       <c r="F111" s="19"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A113" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="17"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A119" s="9"/>
+      <c r="B119" s="10"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="8"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A120" s="9"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="8"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121" s="9"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="8"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A122" s="9"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="22"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="8"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" s="9"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="8"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B124" s="13"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="17"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F126" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="15"/>
+      <c r="F127" s="16"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="9"/>
+      <c r="B128" s="10"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="22"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="8"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" s="9"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="8"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A130" s="9"/>
+      <c r="B130" s="10"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="8"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="14"/>
+      <c r="E131" s="18"/>
+      <c r="F131" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3125,15 +3333,15 @@
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
-    <col min="3" max="3" width="29.375" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="43.58203125" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -3145,19 +3353,19 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -3169,7 +3377,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3179,7 +3387,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -3199,7 +3407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3209,7 +3417,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -3225,7 +3433,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -3235,7 +3443,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3245,7 +3453,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -3265,7 +3473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -3275,7 +3483,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>74</v>
       </c>
@@ -3287,7 +3495,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -3297,7 +3505,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>73</v>
@@ -3311,7 +3519,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -3321,7 +3529,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="25" t="s">
         <v>67</v>
       </c>
@@ -3331,7 +3539,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -3339,7 +3547,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -3355,7 +3563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
@@ -3371,7 +3579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -3381,7 +3589,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3393,19 +3601,19 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -3417,7 +3625,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -3427,7 +3635,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -3447,7 +3655,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -3457,7 +3665,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>76</v>
       </c>
@@ -3473,7 +3681,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>34</v>
       </c>
@@ -3483,7 +3691,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -3493,7 +3701,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -3513,7 +3721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
@@ -3523,7 +3731,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="10" t="s">
         <v>74</v>
       </c>
@@ -3535,7 +3743,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>30</v>
@@ -3545,7 +3753,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>73</v>
@@ -3559,7 +3767,7 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>34</v>
@@ -3569,7 +3777,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="25" t="s">
         <v>67</v>
       </c>
@@ -3579,7 +3787,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="3"/>
@@ -3587,7 +3795,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>37</v>
       </c>
@@ -3603,7 +3811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>39</v>
       </c>
@@ -3619,7 +3827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>34</v>
       </c>
@@ -3629,43 +3837,43 @@
       <c r="E43" s="18"/>
       <c r="F43" s="19"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3675,7 +3883,7 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>26</v>
       </c>
@@ -3695,7 +3903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
@@ -3705,7 +3913,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>76</v>
       </c>
@@ -3721,7 +3929,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>34</v>
       </c>
@@ -3731,7 +3939,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>35</v>
       </c>
@@ -3741,7 +3949,7 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>26</v>
       </c>
@@ -3761,7 +3969,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>30</v>
       </c>
@@ -3771,7 +3979,7 @@
       <c r="E56" s="15"/>
       <c r="F56" s="16"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="10" t="s">
         <v>74</v>
       </c>
@@ -3783,7 +3991,7 @@
       <c r="E57" s="17"/>
       <c r="F57" s="8"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="9"/>
       <c r="B58" s="10" t="s">
         <v>30</v>
@@ -3793,7 +4001,7 @@
       <c r="E58" s="17"/>
       <c r="F58" s="8"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="9"/>
       <c r="B59" s="10" t="s">
         <v>73</v>
@@ -3807,7 +4015,7 @@
       </c>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="9"/>
       <c r="B60" s="10" t="s">
         <v>34</v>
@@ -3817,7 +4025,7 @@
       <c r="E60" s="17"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="25" t="s">
         <v>67</v>
       </c>
@@ -3827,7 +4035,7 @@
       <c r="E61" s="17"/>
       <c r="F61" s="8"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="3"/>
@@ -3835,7 +4043,7 @@
       <c r="E62" s="17"/>
       <c r="F62" s="8"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>37</v>
       </c>
@@ -3851,7 +4059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>39</v>
       </c>
@@ -3867,7 +4075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>34</v>
       </c>
@@ -3877,43 +4085,43 @@
       <c r="E65" s="18"/>
       <c r="F65" s="19"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
@@ -3923,7 +4131,7 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>26</v>
       </c>
@@ -3943,7 +4151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>30</v>
       </c>
@@ -3953,7 +4161,7 @@
       <c r="E73" s="7"/>
       <c r="F73" s="8"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="9" t="s">
         <v>76</v>
       </c>
@@ -3969,7 +4177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>34</v>
       </c>
@@ -3979,7 +4187,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="8"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>35</v>
       </c>
@@ -3989,7 +4197,7 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>26</v>
       </c>
@@ -4009,7 +4217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>30</v>
       </c>
@@ -4019,7 +4227,7 @@
       <c r="E78" s="15"/>
       <c r="F78" s="16"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="10" t="s">
         <v>74</v>
       </c>
@@ -4031,7 +4239,7 @@
       <c r="E79" s="17"/>
       <c r="F79" s="8"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="9"/>
       <c r="B80" s="10" t="s">
         <v>30</v>
@@ -4041,7 +4249,7 @@
       <c r="E80" s="17"/>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="9"/>
       <c r="B81" s="10" t="s">
         <v>73</v>
@@ -4055,7 +4263,7 @@
       </c>
       <c r="F81" s="8"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="9"/>
       <c r="B82" s="10" t="s">
         <v>34</v>
@@ -4065,7 +4273,7 @@
       <c r="E82" s="17"/>
       <c r="F82" s="8"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="25" t="s">
         <v>67</v>
       </c>
@@ -4075,7 +4283,7 @@
       <c r="E83" s="17"/>
       <c r="F83" s="8"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="3"/>
@@ -4083,7 +4291,7 @@
       <c r="E84" s="17"/>
       <c r="F84" s="8"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="9" t="s">
         <v>37</v>
       </c>
@@ -4099,7 +4307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="9" t="s">
         <v>39</v>
       </c>
@@ -4115,7 +4323,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>34</v>
       </c>
@@ -4136,44 +4344,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.125" customWidth="1"/>
-    <col min="3" max="3" width="33.875" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="16.08203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>187</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -4185,9 +4393,9 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4195,7 +4403,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -4215,7 +4423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4225,7 +4433,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>74</v>
       </c>
@@ -4236,28 +4444,28 @@
       <c r="E7" s="17"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="17"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>71</v>
@@ -4266,157 +4474,157 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="E10" s="17" t="s">
         <v>184</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>186</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>91</v>
-      </c>
       <c r="E13" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>171</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>173</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>66</v>
@@ -4428,7 +4636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9"/>
       <c r="B19" s="10" t="s">
         <v>34</v>
@@ -4438,7 +4646,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="25" t="s">
         <v>67</v>
       </c>
@@ -4448,7 +4656,7 @@
       <c r="E20" s="17"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>34</v>
       </c>
@@ -4458,9 +4666,9 @@
       <c r="E21" s="18"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -4468,7 +4676,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -4488,14 +4696,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="3"/>
@@ -4509,7 +4717,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
@@ -4525,7 +4733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>34</v>
       </c>
@@ -4535,45 +4743,45 @@
       <c r="E27" s="14"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4581,7 +4789,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -4601,7 +4809,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
@@ -4611,7 +4819,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="10" t="s">
         <v>74</v>
       </c>
@@ -4623,7 +4831,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>30</v>
@@ -4633,14 +4841,14 @@
       <c r="E36" s="17"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>71</v>
@@ -4649,7 +4857,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>34</v>
@@ -4659,7 +4867,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="25" t="s">
         <v>67</v>
       </c>
@@ -4669,7 +4877,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>34</v>
       </c>
@@ -4679,9 +4887,9 @@
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4689,7 +4897,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>26</v>
       </c>
@@ -4709,14 +4917,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="3"/>
@@ -4730,7 +4938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>39</v>
       </c>
@@ -4746,7 +4954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>34</v>
       </c>
@@ -4766,54 +4974,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="5" width="11.375" customWidth="1"/>
+    <col min="4" max="5" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -4823,7 +5031,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -4843,7 +5051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4853,23 +5061,23 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -4879,7 +5087,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -4889,7 +5097,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -4909,7 +5117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -4919,7 +5127,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>74</v>
       </c>
@@ -4931,7 +5139,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -4941,7 +5149,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>73</v>
@@ -4955,7 +5163,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -4965,7 +5173,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="25" t="s">
         <v>67</v>
       </c>
@@ -4975,7 +5183,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
@@ -4983,7 +5191,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -4999,7 +5207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>39</v>
       </c>
@@ -5015,7 +5223,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -5025,31 +5233,31 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -5061,7 +5269,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -5071,7 +5279,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -5091,7 +5299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -5101,23 +5309,23 @@
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
@@ -5127,7 +5335,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -5137,7 +5345,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>26</v>
       </c>
@@ -5157,7 +5365,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
@@ -5167,7 +5375,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>74</v>
       </c>
@@ -5179,7 +5387,7 @@
       <c r="E34" s="17"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
         <v>30</v>
@@ -5189,7 +5397,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>73</v>
@@ -5203,7 +5411,7 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>34</v>
@@ -5213,7 +5421,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="25" t="s">
         <v>67</v>
       </c>
@@ -5223,7 +5431,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="3"/>
@@ -5231,7 +5439,7 @@
       <c r="E39" s="17"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>37</v>
       </c>
@@ -5247,7 +5455,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>39</v>
       </c>
@@ -5263,7 +5471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>34</v>
       </c>
@@ -5273,43 +5481,43 @@
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +5527,7 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>26</v>
       </c>
@@ -5339,7 +5547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>30</v>
       </c>
@@ -5349,7 +5557,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>53</v>
       </c>
@@ -5365,7 +5573,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>55</v>
       </c>
@@ -5381,7 +5589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>56</v>
       </c>
@@ -5397,7 +5605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>58</v>
       </c>
@@ -5413,7 +5621,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>34</v>
       </c>
@@ -5423,7 +5631,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="17"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
@@ -5433,7 +5641,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>26</v>
       </c>
@@ -5453,7 +5661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -5463,7 +5671,7 @@
       <c r="E58" s="15"/>
       <c r="F58" s="16"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="3"/>
@@ -5471,9 +5679,9 @@
       <c r="E59" s="17"/>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3"/>
@@ -5487,7 +5695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>37</v>
       </c>
@@ -5503,7 +5711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>34</v>
       </c>
@@ -5513,43 +5721,43 @@
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
@@ -5559,7 +5767,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>26</v>
       </c>
@@ -5579,7 +5787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>30</v>
       </c>
@@ -5589,7 +5797,7 @@
       <c r="E70" s="11"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>50</v>
       </c>
@@ -5605,7 +5813,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>34</v>
       </c>
@@ -5615,7 +5823,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>35</v>
       </c>
@@ -5625,7 +5833,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
@@ -5645,7 +5853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>30</v>
       </c>
@@ -5655,7 +5863,7 @@
       <c r="E75" s="15"/>
       <c r="F75" s="16"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="9" t="s">
         <v>37</v>
       </c>
@@ -5671,7 +5879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="9" t="s">
         <v>39</v>
       </c>
@@ -5687,7 +5895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>34</v>
       </c>
@@ -5697,31 +5905,31 @@
       <c r="E78" s="18"/>
       <c r="F78" s="19"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>23</v>
       </c>
@@ -5733,7 +5941,7 @@
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>25</v>
       </c>
@@ -5743,7 +5951,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>26</v>
       </c>
@@ -5763,7 +5971,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>30</v>
       </c>
@@ -5773,23 +5981,23 @@
       <c r="E86" s="7"/>
       <c r="F86" s="8"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E87" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>34</v>
       </c>
@@ -5799,7 +6007,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="8"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>35</v>
       </c>
@@ -5809,7 +6017,7 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>26</v>
       </c>
@@ -5829,7 +6037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>30</v>
       </c>
@@ -5839,7 +6047,7 @@
       <c r="E91" s="15"/>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="10" t="s">
         <v>74</v>
       </c>
@@ -5851,7 +6059,7 @@
       <c r="E92" s="17"/>
       <c r="F92" s="8"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="9"/>
       <c r="B93" s="10" t="s">
         <v>30</v>
@@ -5861,14 +6069,14 @@
       <c r="E93" s="17"/>
       <c r="F93" s="8"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E94" s="17" t="s">
         <v>71</v>
@@ -5877,39 +6085,39 @@
         <v>72</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C95" s="30"/>
       <c r="D95" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="9"/>
       <c r="B96" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C96" s="30"/>
       <c r="D96" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E96" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="9"/>
       <c r="B97" s="10" t="s">
         <v>34</v>
@@ -5919,7 +6127,7 @@
       <c r="E97" s="17"/>
       <c r="F97" s="8"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="25" t="s">
         <v>67</v>
       </c>
@@ -5929,7 +6137,7 @@
       <c r="E98" s="17"/>
       <c r="F98" s="8"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="3"/>
@@ -5937,7 +6145,7 @@
       <c r="E99" s="17"/>
       <c r="F99" s="8"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="9" t="s">
         <v>37</v>
       </c>
@@ -5953,7 +6161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="9" t="s">
         <v>39</v>
       </c>
@@ -5969,7 +6177,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>34</v>
       </c>
@@ -5979,31 +6187,31 @@
       <c r="E102" s="18"/>
       <c r="F102" s="19"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>23</v>
       </c>
@@ -6015,7 +6223,7 @@
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>25</v>
       </c>
@@ -6025,7 +6233,7 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>26</v>
       </c>
@@ -6045,7 +6253,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>30</v>
       </c>
@@ -6055,23 +6263,23 @@
       <c r="E109" s="7"/>
       <c r="F109" s="8"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E110" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F110" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>34</v>
       </c>
@@ -6081,7 +6289,7 @@
       <c r="E111" s="14"/>
       <c r="F111" s="8"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>35</v>
       </c>
@@ -6091,7 +6299,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>26</v>
       </c>
@@ -6111,7 +6319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>30</v>
       </c>
@@ -6121,7 +6329,7 @@
       <c r="E114" s="15"/>
       <c r="F114" s="16"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="3"/>
@@ -6129,7 +6337,7 @@
       <c r="E115" s="17"/>
       <c r="F115" s="8"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="9"/>
       <c r="B116" s="10"/>
       <c r="C116" s="3"/>
@@ -6137,7 +6345,7 @@
       <c r="E116" s="17"/>
       <c r="F116" s="8"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="9"/>
       <c r="B117" s="10"/>
       <c r="C117" s="3"/>
@@ -6145,7 +6353,7 @@
       <c r="E117" s="17"/>
       <c r="F117" s="8"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="9"/>
       <c r="B118" s="10"/>
       <c r="C118" s="30"/>
@@ -6153,7 +6361,7 @@
       <c r="E118" s="17"/>
       <c r="F118" s="8"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="9"/>
       <c r="B119" s="10"/>
       <c r="C119" s="30"/>
@@ -6161,7 +6369,7 @@
       <c r="E119" s="24"/>
       <c r="F119" s="8"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="9"/>
       <c r="B120" s="10"/>
       <c r="C120" s="3"/>
@@ -6169,7 +6377,7 @@
       <c r="E120" s="17"/>
       <c r="F120" s="8"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="25"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -6177,7 +6385,7 @@
       <c r="E121" s="17"/>
       <c r="F121" s="8"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
       <c r="C122" s="3"/>
@@ -6185,7 +6393,7 @@
       <c r="E122" s="17"/>
       <c r="F122" s="8"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="9" t="s">
         <v>37</v>
       </c>
@@ -6201,7 +6409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="9" t="s">
         <v>39</v>
       </c>
@@ -6217,7 +6425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>34</v>
       </c>
@@ -6242,40 +6450,40 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.375" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1"/>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -6287,7 +6495,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -6297,7 +6505,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -6317,7 +6525,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -6327,14 +6535,14 @@
       <c r="E6" s="7"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>44</v>
@@ -6343,30 +6551,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>71</v>
@@ -6375,7 +6583,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="9"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6383,7 +6591,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6391,7 +6599,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
@@ -6401,7 +6609,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -6411,7 +6619,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -6431,7 +6639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -6441,9 +6649,9 @@
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="3"/>
@@ -6451,20 +6659,20 @@
         <v>46</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>32</v>
@@ -6473,14 +6681,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="3"/>
       <c r="D18" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>62</v>
@@ -6489,7 +6697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
@@ -6499,7 +6707,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>34</v>
       </c>
@@ -6509,43 +6717,43 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -6555,7 +6763,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -6575,7 +6783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -6585,14 +6793,14 @@
       <c r="E28" s="7"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>71</v>
@@ -6601,7 +6809,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="9"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6609,7 +6817,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="9"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6617,7 +6825,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="9"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6625,7 +6833,7 @@
       <c r="E32" s="11"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="9"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6633,7 +6841,7 @@
       <c r="E33" s="11"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>34</v>
       </c>
@@ -6643,7 +6851,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -6653,7 +6861,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
@@ -6673,7 +6881,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>30</v>
       </c>
@@ -6683,9 +6891,9 @@
       <c r="E37" s="15"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="3"/>
@@ -6693,20 +6901,20 @@
         <v>46</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="3"/>
       <c r="D39" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>32</v>
@@ -6715,7 +6923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="3"/>
@@ -6723,7 +6931,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>34</v>
       </c>
@@ -6733,43 +6941,43 @@
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -6779,7 +6987,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>26</v>
       </c>
@@ -6799,7 +7007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>30</v>
       </c>
@@ -6809,14 +7017,14 @@
       <c r="E48" s="7"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="3"/>
       <c r="D49" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>44</v>
@@ -6825,23 +7033,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="9"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -6849,7 +7057,7 @@
       <c r="E51" s="11"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="9"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -6857,7 +7065,7 @@
       <c r="E52" s="11"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="9"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6865,7 +7073,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>34</v>
       </c>
@@ -6875,7 +7083,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="17"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
@@ -6885,7 +7093,7 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>26</v>
       </c>
@@ -6905,7 +7113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>30</v>
       </c>
@@ -6915,9 +7123,9 @@
       <c r="E57" s="15"/>
       <c r="F57" s="16"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="3"/>
@@ -6925,20 +7133,20 @@
         <v>46</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="3"/>
       <c r="D59" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>32</v>
@@ -6947,7 +7155,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="3"/>
@@ -6955,7 +7163,7 @@
       <c r="E60" s="17"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>34</v>
       </c>

</xml_diff>